<commit_message>
coding the daly weights in conjunction with healthburden
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Oesophageal_Cancer.xlsx
+++ b/resources/ResourceFile_Oesophageal_Cancer.xlsx
@@ -783,7 +783,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -871,7 +871,7 @@
         <xdr:cNvPr id="43" name="Oval 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00002B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1040,7 +1040,7 @@
         <xdr:cNvPr id="44" name="TextBox 140">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00002C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1196,7 +1196,7 @@
         <xdr:cNvPr id="45" name="Straight Arrow Connector 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1255,7 +1255,7 @@
         <xdr:cNvPr id="46" name="Rectangle 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00002E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1397,7 +1397,7 @@
         <xdr:cNvPr id="47" name="Oval 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00002F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1566,7 +1566,7 @@
         <xdr:cNvPr id="48" name="TextBox 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000030000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000030000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1710,7 +1710,7 @@
         <xdr:cNvPr id="49" name="TextBox 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000031000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000031000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1854,7 +1854,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1898,7 +1898,7 @@
         <xdr:cNvPr id="90" name="Picture 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00005A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-00005A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1948,7 +1948,7 @@
         <xdr:cNvPr id="97" name="Picture 96">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000061000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0100-000061000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2003,7 +2003,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2064,7 +2064,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2125,7 +2125,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2186,7 +2186,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2247,7 +2247,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2308,7 +2308,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" xmlns="" id="{00000000-0008-0000-0300-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -3431,7 +3431,7 @@
   <dimension ref="A1:J36"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>

</xml_diff>

<commit_message>
Use load_parameters_from_dataframe method with oesophageal cancer module
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Oesophageal_Cancer.xlsx
+++ b/resources/ResourceFile_Oesophageal_Cancer.xlsx
@@ -1,15 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" mc:Ignorable="x15">
-  <fileVersion appName="xl" lastEdited="6" lowestEdited="6" rupBuild="14420"/>
-  <workbookPr/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="10715"/>
+  <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Andrew Phillips\PycharmProjects\TLOmodel\resources\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/stef/UCL/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C2AC7B48-2C9F-DB4D-A2AD-01947DE8F11D}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="340" yWindow="780" windowWidth="25460" windowHeight="15720" activeTab="2"/>
+    <workbookView xWindow="14760" yWindow="-22580" windowWidth="38400" windowHeight="21140" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Cover Sheet" sheetId="1" r:id="rId1"/>
@@ -17,17 +18,23 @@
     <sheet name="parameter_values" sheetId="3" r:id="rId3"/>
     <sheet name="additional info" sheetId="7" r:id="rId4"/>
   </sheets>
-  <calcPr calcId="152511"/>
+  <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
+    </ext>
+    <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
+      <xcalcf:calcFeatures>
+        <xcalcf:feature name="microsoft.com:RD"/>
+        <xcalcf:feature name="microsoft.com:FV"/>
+      </xcalcf:calcFeatures>
     </ext>
   </extLst>
 </workbook>
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="203" uniqueCount="144">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="205" uniqueCount="146">
   <si>
     <t>Name:</t>
   </si>
@@ -461,21 +468,6 @@
     <t>r_high_grade_dysplasia_low_grade_dysp</t>
   </si>
   <si>
-    <t>value2</t>
-  </si>
-  <si>
-    <t>value3</t>
-  </si>
-  <si>
-    <t>value4</t>
-  </si>
-  <si>
-    <t>value5</t>
-  </si>
-  <si>
-    <t>value6</t>
-  </si>
-  <si>
     <t>probability per 3 months of diagnosis in a person with stage 1 oesophageal cancer</t>
   </si>
   <si>
@@ -483,12 +475,33 @@
   </si>
   <si>
     <t>rate ratio for diagnosis if have high grade oesophageal dysplasia</t>
+  </si>
+  <si>
+    <t>[0.0003, 0.0001, 0.000005, 0.00003, 0.00005, 0.00001]</t>
+  </si>
+  <si>
+    <t>[0.01, 0.03, 0.1, 0.2, 0.3, 0.8]</t>
+  </si>
+  <si>
+    <t>[0.01, 0.01, 0.05, 0.05, 0.05, 0.05]</t>
+  </si>
+  <si>
+    <t>daly_wt_oes_cancer_controlled</t>
+  </si>
+  <si>
+    <t>daly_wt_oes_cancer_terminal</t>
+  </si>
+  <si>
+    <t>daly_wt_oes_cancer_metastatic</t>
+  </si>
+  <si>
+    <t>daly_wt_oes_cancer_primary_therapy</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <fonts count="10" x14ac:knownFonts="1">
     <font>
       <sz val="12"/>
@@ -783,7 +796,7 @@
         <xdr:cNvPr id="2" name="TextBox 1">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000002000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -871,7 +884,7 @@
         <xdr:cNvPr id="43" name="Oval 42">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002B000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002B000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1040,7 +1053,7 @@
         <xdr:cNvPr id="44" name="TextBox 140">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002C000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002C000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1196,7 +1209,7 @@
         <xdr:cNvPr id="45" name="Straight Arrow Connector 44">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002D000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002D000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1255,7 +1268,7 @@
         <xdr:cNvPr id="46" name="Rectangle 45">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002E000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002E000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1397,7 +1410,7 @@
         <xdr:cNvPr id="47" name="Oval 46">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002F000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00002F000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1566,7 +1579,7 @@
         <xdr:cNvPr id="48" name="TextBox 25">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000030000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000030000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1710,7 +1723,7 @@
         <xdr:cNvPr id="49" name="TextBox 26">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000031000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000031000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1854,7 +1867,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1898,7 +1911,7 @@
         <xdr:cNvPr id="90" name="Picture 89">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00005A000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-00005A000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -1948,7 +1961,7 @@
         <xdr:cNvPr id="97" name="Picture 96">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000061000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0100-000061000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2003,7 +2016,7 @@
         <xdr:cNvPr id="3" name="Picture 2">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000003000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2064,7 +2077,7 @@
         <xdr:cNvPr id="4" name="Picture 3">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000004000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2125,7 +2138,7 @@
         <xdr:cNvPr id="5" name="Picture 4">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000005000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2186,7 +2199,7 @@
         <xdr:cNvPr id="6" name="Picture 5">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000006000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2247,7 +2260,7 @@
         <xdr:cNvPr id="7" name="Picture 6">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000007000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2308,7 +2321,7 @@
         <xdr:cNvPr id="8" name="Picture 7">
           <a:extLst>
             <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
-              <a16:creationId xmlns="" xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{00000000-0008-0000-0300-000008000000}"/>
             </a:ext>
           </a:extLst>
         </xdr:cNvPr>
@@ -2650,20 +2663,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="B3:C28"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C30" sqref="C29:C30"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="34.1640625" customWidth="1"/>
     <col min="3" max="3" width="90.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="3" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B3" s="9" t="s">
         <v>0</v>
       </c>
@@ -2671,10 +2684,10 @@
         <v>26</v>
       </c>
     </row>
-    <row r="4" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B4" s="2"/>
     </row>
-    <row r="5" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B5" s="9" t="s">
         <v>3</v>
       </c>
@@ -2682,19 +2695,19 @@
         <v>120</v>
       </c>
     </row>
-    <row r="6" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B6" s="7" t="s">
         <v>13</v>
       </c>
       <c r="C6" s="8"/>
     </row>
-    <row r="7" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B7" s="2"/>
       <c r="C7" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="8" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B8" s="9" t="s">
         <v>1</v>
       </c>
@@ -2702,10 +2715,10 @@
         <v>27</v>
       </c>
     </row>
-    <row r="9" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B9" s="2"/>
     </row>
-    <row r="10" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B10" s="9" t="s">
         <v>2</v>
       </c>
@@ -2713,10 +2726,10 @@
         <v>14</v>
       </c>
     </row>
-    <row r="11" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B11" s="2"/>
     </row>
-    <row r="12" spans="2:3" ht="95" customHeight="1" x14ac:dyDescent="0.35">
+    <row r="12" spans="2:3" ht="95" customHeight="1" x14ac:dyDescent="0.2">
       <c r="B12" s="10" t="s">
         <v>4</v>
       </c>
@@ -2724,7 +2737,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="14" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="14" spans="2:3" ht="34" x14ac:dyDescent="0.2">
       <c r="B14" s="11" t="s">
         <v>24</v>
       </c>
@@ -2732,19 +2745,19 @@
         <v>121</v>
       </c>
     </row>
-    <row r="15" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="15" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B15" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C15" s="6"/>
     </row>
-    <row r="16" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B16" s="5" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="6"/>
     </row>
-    <row r="17" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="17" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B17" s="5" t="s">
         <v>7</v>
       </c>
@@ -2752,13 +2765,13 @@
         <v>122</v>
       </c>
     </row>
-    <row r="18" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="18" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B18" s="5" t="s">
         <v>10</v>
       </c>
       <c r="C18" s="6"/>
     </row>
-    <row r="19" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="19" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B19" s="5" t="s">
         <v>9</v>
       </c>
@@ -2766,25 +2779,25 @@
         <v>121</v>
       </c>
     </row>
-    <row r="20" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="20" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B20" s="7" t="s">
         <v>8</v>
       </c>
       <c r="C20" s="8"/>
     </row>
-    <row r="22" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="22" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B22" s="12" t="s">
         <v>25</v>
       </c>
       <c r="C22" s="4"/>
     </row>
-    <row r="23" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="23" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B23" s="5" t="s">
         <v>5</v>
       </c>
       <c r="C23" s="20"/>
     </row>
-    <row r="24" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="24" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B24" s="5" t="s">
         <v>6</v>
       </c>
@@ -2792,7 +2805,7 @@
         <v>123</v>
       </c>
     </row>
-    <row r="25" spans="2:3" ht="31" x14ac:dyDescent="0.35">
+    <row r="25" spans="2:3" ht="34" x14ac:dyDescent="0.2">
       <c r="B25" s="5" t="s">
         <v>7</v>
       </c>
@@ -2800,7 +2813,7 @@
         <v>126</v>
       </c>
     </row>
-    <row r="26" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="26" spans="2:3" ht="17" x14ac:dyDescent="0.2">
       <c r="B26" s="13" t="s">
         <v>10</v>
       </c>
@@ -2808,7 +2821,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="27" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="27" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B27" t="s">
         <v>9</v>
       </c>
@@ -2816,7 +2829,7 @@
         <v>124</v>
       </c>
     </row>
-    <row r="28" spans="2:3" x14ac:dyDescent="0.35">
+    <row r="28" spans="2:3" x14ac:dyDescent="0.2">
       <c r="B28" t="s">
         <v>8</v>
       </c>
@@ -2831,27 +2844,27 @@
 </file>
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0100-000000000000}">
   <dimension ref="A37:F91"/>
   <sheetViews>
     <sheetView topLeftCell="A53" zoomScale="80" zoomScaleNormal="80" workbookViewId="0">
       <selection activeCell="B80" sqref="B80"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="2" max="2" width="47.83203125" customWidth="1"/>
     <col min="3" max="3" width="55.1640625" customWidth="1"/>
     <col min="4" max="4" width="127.6640625" customWidth="1"/>
-    <col min="5" max="5" width="150.9140625" style="29" customWidth="1"/>
+    <col min="5" max="5" width="150.83203125" style="29" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="37" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="37" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B37" s="1" t="s">
         <v>11</v>
       </c>
     </row>
-    <row r="39" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="39" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B39" s="1" t="s">
         <v>19</v>
       </c>
@@ -2860,7 +2873,7 @@
       </c>
       <c r="E39" s="1"/>
     </row>
-    <row r="40" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="40" spans="2:5" ht="17" x14ac:dyDescent="0.2">
       <c r="B40" t="s">
         <v>31</v>
       </c>
@@ -2868,7 +2881,7 @@
         <v>36</v>
       </c>
     </row>
-    <row r="41" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="41" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B41" t="s">
         <v>32</v>
       </c>
@@ -2876,7 +2889,7 @@
         <v>35</v>
       </c>
     </row>
-    <row r="42" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B42" t="s">
         <v>33</v>
       </c>
@@ -2884,7 +2897,7 @@
         <v>34</v>
       </c>
     </row>
-    <row r="43" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="43" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B43" t="s">
         <v>118</v>
       </c>
@@ -2892,12 +2905,12 @@
         <v>119</v>
       </c>
     </row>
-    <row r="45" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="45" spans="2:5" x14ac:dyDescent="0.2">
       <c r="C45" t="s">
         <v>122</v>
       </c>
     </row>
-    <row r="46" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="46" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B46" s="1" t="s">
         <v>16</v>
       </c>
@@ -2911,7 +2924,7 @@
         <v>12</v>
       </c>
     </row>
-    <row r="47" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="47" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B47" t="s">
         <v>98</v>
       </c>
@@ -2925,7 +2938,7 @@
         <v>55</v>
       </c>
     </row>
-    <row r="48" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="48" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B48" t="s">
         <v>37</v>
       </c>
@@ -2939,7 +2952,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="49" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="49" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B49" t="s">
         <v>38</v>
       </c>
@@ -2953,7 +2966,7 @@
         <v>54</v>
       </c>
     </row>
-    <row r="50" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="50" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B50" s="23" t="s">
         <v>39</v>
       </c>
@@ -2967,7 +2980,7 @@
         <v>53</v>
       </c>
     </row>
-    <row r="51" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="51" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B51" t="s">
         <v>40</v>
       </c>
@@ -2981,7 +2994,7 @@
         <v>52</v>
       </c>
     </row>
-    <row r="52" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="52" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B52" t="s">
         <v>99</v>
       </c>
@@ -2995,7 +3008,7 @@
         <v>59</v>
       </c>
     </row>
-    <row r="53" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="53" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B53" s="24" t="s">
         <v>107</v>
       </c>
@@ -3012,7 +3025,7 @@
         <v>122</v>
       </c>
     </row>
-    <row r="54" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="54" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B54" t="s">
         <v>100</v>
       </c>
@@ -3026,7 +3039,7 @@
         <v>60</v>
       </c>
     </row>
-    <row r="55" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="55" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B55" t="s">
         <v>107</v>
       </c>
@@ -3040,7 +3053,7 @@
         <v>65</v>
       </c>
     </row>
-    <row r="56" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="56" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B56" s="23" t="s">
         <v>101</v>
       </c>
@@ -3054,7 +3067,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="57" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="57" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B57" s="23" t="s">
         <v>108</v>
       </c>
@@ -3068,7 +3081,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="58" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="58" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B58" s="23" t="s">
         <v>102</v>
       </c>
@@ -3082,7 +3095,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="59" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="59" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B59" s="23" t="s">
         <v>109</v>
       </c>
@@ -3096,7 +3109,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="60" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="60" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B60" s="27" t="s">
         <v>103</v>
       </c>
@@ -3110,7 +3123,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="61" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="61" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B61" s="27" t="s">
         <v>110</v>
       </c>
@@ -3124,7 +3137,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="62" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="62" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B62" s="23" t="s">
         <v>105</v>
       </c>
@@ -3138,7 +3151,7 @@
         <v>62</v>
       </c>
     </row>
-    <row r="63" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="63" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B63" s="23" t="s">
         <v>104</v>
       </c>
@@ -3152,7 +3165,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="64" spans="2:6" x14ac:dyDescent="0.35">
+    <row r="64" spans="2:6" x14ac:dyDescent="0.2">
       <c r="B64" s="23" t="s">
         <v>45</v>
       </c>
@@ -3166,7 +3179,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="65" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="65" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B65" s="23" t="s">
         <v>66</v>
       </c>
@@ -3180,7 +3193,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="66" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="66" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B66" s="23" t="s">
         <v>67</v>
       </c>
@@ -3194,7 +3207,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="67" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="67" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B67" s="23" t="s">
         <v>68</v>
       </c>
@@ -3208,7 +3221,7 @@
         <v>57</v>
       </c>
     </row>
-    <row r="68" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="68" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B68" s="28" t="s">
         <v>131</v>
       </c>
@@ -3216,13 +3229,13 @@
         <v>0.01</v>
       </c>
       <c r="D68" t="s">
-        <v>141</v>
+        <v>136</v>
       </c>
       <c r="E68" s="16" t="s">
         <v>64</v>
       </c>
     </row>
-    <row r="69" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="69" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B69" s="28" t="s">
         <v>130</v>
       </c>
@@ -3230,13 +3243,13 @@
         <v>0.01</v>
       </c>
       <c r="D69" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="E69" s="16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="70" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="70" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B70" s="28" t="s">
         <v>46</v>
       </c>
@@ -3244,13 +3257,13 @@
         <v>0.01</v>
       </c>
       <c r="D70" t="s">
-        <v>143</v>
+        <v>138</v>
       </c>
       <c r="E70" s="16" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="71" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="71" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B71" s="28" t="s">
         <v>69</v>
       </c>
@@ -3264,7 +3277,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="72" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="72" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B72" s="28" t="s">
         <v>70</v>
       </c>
@@ -3278,7 +3291,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="73" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="73" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B73" s="28" t="s">
         <v>71</v>
       </c>
@@ -3292,7 +3305,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="74" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="74" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B74" s="28" t="s">
         <v>106</v>
       </c>
@@ -3304,7 +3317,7 @@
       </c>
       <c r="E74" s="16"/>
     </row>
-    <row r="75" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="75" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B75" s="28" t="s">
         <v>91</v>
       </c>
@@ -3318,7 +3331,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="76" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="76" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B76" s="28" t="s">
         <v>88</v>
       </c>
@@ -3332,7 +3345,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="77" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="77" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B77" s="28" t="s">
         <v>112</v>
       </c>
@@ -3346,7 +3359,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="78" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="78" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B78" s="28" t="s">
         <v>113</v>
       </c>
@@ -3360,7 +3373,7 @@
         <v>116</v>
       </c>
     </row>
-    <row r="79" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="79" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B79" s="30" t="s">
         <v>92</v>
       </c>
@@ -3372,7 +3385,7 @@
       </c>
       <c r="E79" s="16"/>
     </row>
-    <row r="80" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="80" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B80" s="28" t="s">
         <v>95</v>
       </c>
@@ -3383,7 +3396,7 @@
         <v>96</v>
       </c>
     </row>
-    <row r="82" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="82" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B82" s="23"/>
       <c r="C82" t="s">
         <v>122</v>
@@ -3392,7 +3405,7 @@
         <v>87</v>
       </c>
     </row>
-    <row r="84" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="84" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B84" s="1" t="s">
         <v>30</v>
       </c>
@@ -3403,19 +3416,19 @@
         <v>61</v>
       </c>
     </row>
-    <row r="88" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="88" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A88" s="15"/>
       <c r="D88" s="15"/>
     </row>
-    <row r="89" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="89" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A89" s="15"/>
       <c r="D89" s="15"/>
     </row>
-    <row r="90" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="90" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A90" s="15"/>
       <c r="D90" s="15"/>
     </row>
-    <row r="91" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="91" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A91" s="15"/>
       <c r="D91" s="15"/>
     </row>
@@ -3427,14 +3440,14 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:J36"/>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0200-000000000000}">
+  <dimension ref="A1:J39"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A4" workbookViewId="0">
-      <selection activeCell="A21" sqref="A21"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="A23" sqref="A23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="60.5" customWidth="1"/>
     <col min="3" max="3" width="19.1640625" customWidth="1"/>
@@ -3442,33 +3455,23 @@
     <col min="5" max="5" width="13.83203125" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>127</v>
       </c>
       <c r="B1" s="1" t="s">
         <v>128</v>
       </c>
-      <c r="C1" s="1" t="s">
-        <v>136</v>
-      </c>
-      <c r="D1" s="1" t="s">
-        <v>137</v>
-      </c>
-      <c r="E1" s="1" t="s">
-        <v>138</v>
-      </c>
-      <c r="F1" s="1" t="s">
-        <v>139</v>
-      </c>
-      <c r="G1" s="1" t="s">
-        <v>140</v>
-      </c>
+      <c r="C1" s="1"/>
+      <c r="D1" s="1"/>
+      <c r="E1" s="1"/>
+      <c r="F1" s="1"/>
+      <c r="G1" s="1"/>
       <c r="H1" s="1"/>
       <c r="I1" s="1"/>
       <c r="J1" s="1"/>
     </row>
-    <row r="2" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A2" s="32" t="s">
         <v>98</v>
       </c>
@@ -3476,7 +3479,7 @@
         <v>0.5</v>
       </c>
     </row>
-    <row r="3" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A3" s="32" t="s">
         <v>37</v>
       </c>
@@ -3484,7 +3487,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="4" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A4" s="32" t="s">
         <v>38</v>
       </c>
@@ -3493,7 +3496,7 @@
       </c>
       <c r="I4" s="14"/>
     </row>
-    <row r="5" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A5" s="32" t="s">
         <v>39</v>
       </c>
@@ -3502,7 +3505,7 @@
       </c>
       <c r="I5" s="14"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A6" s="32" t="s">
         <v>40</v>
       </c>
@@ -3511,7 +3514,7 @@
       </c>
       <c r="I6" s="14"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A7" s="32" t="s">
         <v>135</v>
       </c>
@@ -3520,7 +3523,7 @@
       </c>
       <c r="I7" s="14"/>
     </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A8" s="32" t="s">
         <v>107</v>
       </c>
@@ -3528,7 +3531,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="9" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A9" s="32" t="s">
         <v>134</v>
       </c>
@@ -3536,7 +3539,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A10" s="32" t="s">
         <v>108</v>
       </c>
@@ -3544,7 +3547,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A11" s="32" t="s">
         <v>101</v>
       </c>
@@ -3552,7 +3555,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A12" s="32" t="s">
         <v>109</v>
       </c>
@@ -3560,7 +3563,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A13" s="32" t="s">
         <v>102</v>
       </c>
@@ -3568,7 +3571,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A14" s="32" t="s">
         <v>110</v>
       </c>
@@ -3576,7 +3579,7 @@
         <v>0.1</v>
       </c>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A15" s="32" t="s">
         <v>103</v>
       </c>
@@ -3584,7 +3587,7 @@
         <v>0.05</v>
       </c>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.2">
       <c r="A16" s="32" t="s">
         <v>133</v>
       </c>
@@ -3592,7 +3595,7 @@
         <v>0.3</v>
       </c>
     </row>
-    <row r="17" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A17" s="32" t="s">
         <v>132</v>
       </c>
@@ -3600,7 +3603,7 @@
         <v>0.4</v>
       </c>
     </row>
-    <row r="18" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A18" s="32" t="s">
         <v>104</v>
       </c>
@@ -3608,7 +3611,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="19" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A19" s="32" t="s">
         <v>45</v>
       </c>
@@ -3616,7 +3619,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="20" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A20" s="32" t="s">
         <v>66</v>
       </c>
@@ -3624,7 +3627,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="21" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A21" s="32" t="s">
         <v>67</v>
       </c>
@@ -3632,7 +3635,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="22" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A22" s="32" t="s">
         <v>68</v>
       </c>
@@ -3640,7 +3643,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="23" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="32" t="s">
         <v>131</v>
       </c>
@@ -3648,7 +3651,7 @@
         <v>100</v>
       </c>
     </row>
-    <row r="24" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A24" s="32" t="s">
         <v>130</v>
       </c>
@@ -3656,7 +3659,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="25" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A25" s="32" t="s">
         <v>46</v>
       </c>
@@ -3664,7 +3667,7 @@
         <v>0.01</v>
       </c>
     </row>
-    <row r="26" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A26" s="32" t="s">
         <v>69</v>
       </c>
@@ -3672,7 +3675,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="27" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A27" s="32" t="s">
         <v>70</v>
       </c>
@@ -3680,7 +3683,7 @@
         <v>50</v>
       </c>
     </row>
-    <row r="28" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A28" s="32" t="s">
         <v>71</v>
       </c>
@@ -3688,30 +3691,15 @@
         <v>100</v>
       </c>
     </row>
-    <row r="29" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A29" s="32" t="s">
         <v>106</v>
       </c>
-      <c r="B29">
-        <v>2.9999999999999997E-4</v>
-      </c>
-      <c r="C29">
-        <v>1E-4</v>
-      </c>
-      <c r="D29">
-        <v>5.0000000000000004E-6</v>
-      </c>
-      <c r="E29">
-        <v>3.0000000000000001E-5</v>
-      </c>
-      <c r="F29">
-        <v>5.0000000000000002E-5</v>
-      </c>
-      <c r="G29">
-        <v>1.0000000000000001E-5</v>
-      </c>
-    </row>
-    <row r="30" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B29" t="s">
+        <v>139</v>
+      </c>
+    </row>
+    <row r="30" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A30" s="32" t="s">
         <v>91</v>
       </c>
@@ -3719,7 +3707,7 @@
         <v>1.3</v>
       </c>
     </row>
-    <row r="31" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A31" s="32" t="s">
         <v>88</v>
       </c>
@@ -3727,7 +3715,7 @@
         <v>1.1000000000000001</v>
       </c>
     </row>
-    <row r="32" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="32" t="s">
         <v>113</v>
       </c>
@@ -3735,7 +3723,7 @@
         <v>2</v>
       </c>
     </row>
-    <row r="33" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A33" s="32" t="s">
         <v>112</v>
       </c>
@@ -3743,54 +3731,53 @@
         <v>1</v>
       </c>
     </row>
-    <row r="34" spans="1:7" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A34" s="32" t="s">
         <v>92</v>
       </c>
-      <c r="B34">
-        <v>0.01</v>
-      </c>
-      <c r="C34">
-        <v>0.03</v>
-      </c>
-      <c r="D34">
-        <v>0.1</v>
-      </c>
-      <c r="E34">
-        <v>0.2</v>
-      </c>
-      <c r="F34">
-        <v>0.3</v>
-      </c>
-      <c r="G34">
-        <v>0.8</v>
-      </c>
-    </row>
-    <row r="35" spans="1:7" x14ac:dyDescent="0.35">
+      <c r="B34" t="s">
+        <v>140</v>
+      </c>
+    </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A35" s="32" t="s">
         <v>129</v>
       </c>
-      <c r="B35">
-        <v>0.01</v>
-      </c>
-      <c r="C35">
-        <v>0.01</v>
-      </c>
-      <c r="D35">
-        <v>0.05</v>
-      </c>
-      <c r="E35">
-        <v>0.05</v>
-      </c>
-      <c r="F35">
-        <v>0.05</v>
-      </c>
-      <c r="G35">
-        <v>0.05</v>
-      </c>
-    </row>
-    <row r="36" spans="1:7" x14ac:dyDescent="0.35">
-      <c r="A36" s="16"/>
+      <c r="B35" t="s">
+        <v>141</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>142</v>
+      </c>
+      <c r="B36">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>143</v>
+      </c>
+      <c r="B37">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>144</v>
+      </c>
+      <c r="B38">
+        <v>0</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>145</v>
+      </c>
+      <c r="B39">
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -3799,37 +3786,37 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0300-000000000000}">
   <dimension ref="B4:E598"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="C20" sqref="C20"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultColWidth="10.6640625" defaultRowHeight="15.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <sheetData>
-    <row r="4" spans="2:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="2:5" x14ac:dyDescent="0.2">
       <c r="B4" s="17"/>
       <c r="C4" s="17"/>
       <c r="D4" s="17"/>
       <c r="E4" s="17"/>
     </row>
-    <row r="592" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="592" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B592" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="594" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="594" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B594" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="596" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="596" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B596" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="598" spans="2:2" x14ac:dyDescent="0.35">
+    <row r="598" spans="2:2" x14ac:dyDescent="0.2">
       <c r="B598" t="s">
         <v>18</v>
       </c>

</xml_diff>

<commit_message>
ANALYSIS SCRIPT ALMOST DONE
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Oesophageal_Cancer.xlsx
+++ b/resources/ResourceFile_Oesophageal_Cancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tbh03/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{75A013B0-2320-434E-A9FA-D028E5A98FFD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946759A1-A1A4-F24A-ACD0-A6A5F02FAEBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1020" yWindow="1180" windowWidth="17780" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1040" yWindow="1020" windowWidth="17780" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter_values" sheetId="3" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="40" uniqueCount="40">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="39" uniqueCount="39">
   <si>
     <t>rr_low_grade_dysplasia_none_female</t>
   </si>
@@ -136,9 +136,6 @@
   </si>
   <si>
     <t>sensitivity_of_endoscopy_for_oes_cancer_with_dysphagia</t>
-  </si>
-  <si>
-    <t>prob_present_dysphagia</t>
   </si>
   <si>
     <t>rate_palliative_care_stage4</t>
@@ -538,7 +535,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A2" sqref="A2"/>
+      <selection activeCell="A36" sqref="A36"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -749,7 +746,7 @@
     </row>
     <row r="23" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A23" s="5" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B23">
         <v>0.5</v>
@@ -821,7 +818,7 @@
     </row>
     <row r="32" spans="1:2" x14ac:dyDescent="0.2">
       <c r="A32" s="5" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="B32">
         <v>0.5</v>
@@ -844,12 +841,7 @@
       </c>
     </row>
     <row r="35" spans="1:2" x14ac:dyDescent="0.2">
-      <c r="A35" s="6" t="s">
-        <v>37</v>
-      </c>
-      <c r="B35">
-        <v>0.8</v>
-      </c>
+      <c r="A35" s="6"/>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
plotting scripts in the analyses
</commit_message>
<xml_diff>
--- a/resources/ResourceFile_Oesophageal_Cancer.xlsx
+++ b/resources/ResourceFile_Oesophageal_Cancer.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/tbh03/PycharmProjects/TLOmodel/resources/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{946759A1-A1A4-F24A-ACD0-A6A5F02FAEBD}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D44B002D-CBE0-4D43-98E7-38E8D5BE2F48}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1040" yWindow="1020" windowWidth="17780" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="680" yWindow="1000" windowWidth="17780" windowHeight="17040" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="parameter_values" sheetId="3" r:id="rId1"/>
@@ -535,7 +535,7 @@
   <dimension ref="A1:J35"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A36" sqref="A36"/>
+      <selection activeCell="A18" sqref="A18"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultColWidth="10.6640625" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -717,7 +717,7 @@
         <v>28</v>
       </c>
       <c r="B19">
-        <v>0.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="20" spans="1:2" x14ac:dyDescent="0.2">
@@ -725,7 +725,7 @@
         <v>29</v>
       </c>
       <c r="B20">
-        <v>0.01</v>
+        <v>1</v>
       </c>
     </row>
     <row r="21" spans="1:2" x14ac:dyDescent="0.2">

</xml_diff>